<commit_message>
add maven, apache poi, lombok
</commit_message>
<xml_diff>
--- a/src/main/resources/exportItems.xlsx
+++ b/src/main/resources/exportItems.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>a</t>
   </si>
@@ -23,10 +23,7 @@
     <t>CAR</t>
   </si>
   <si>
-    <t>Fri May 15 09:25:22 MSK 2020</t>
-  </si>
-  <si>
-    <t>Fri May 15 12:59:59 MSK 2020</t>
+    <t>Sat May 16 13:51:18 MSK 2020</t>
   </si>
 </sst>
 </file>
@@ -71,7 +68,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:F3"/>
+  <dimension ref="A2:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -79,7 +76,7 @@
   <sheetData>
     <row r="2">
       <c r="A2" t="n">
-        <v>10.0</v>
+        <v>1.0</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -97,26 +94,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>